<commit_message>
Changed Brave to Brawe. Added More Statistic points to view.
</commit_message>
<xml_diff>
--- a/DATA/10 Mar 2024/Klein Jakkelse.xlsx
+++ b/DATA/10 Mar 2024/Klein Jakkelse.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="15">
   <si>
     <t>ID</t>
   </si>
@@ -39,6 +39,24 @@
   </si>
   <si>
     <t>Eerste</t>
+  </si>
+  <si>
+    <t>TestName2 TestSurname2</t>
+  </si>
+  <si>
+    <t>TestParentName3 TestParentSurname3</t>
+  </si>
+  <si>
+    <t>085 555 6666</t>
+  </si>
+  <si>
+    <t>Tweede</t>
+  </si>
+  <si>
+    <t>TestName3 TestSurname3</t>
+  </si>
+  <si>
+    <t>TestParentName TestParent Surname</t>
   </si>
 </sst>
 </file>
@@ -83,7 +101,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -123,6 +141,91 @@
         <v>8</v>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" t="n" s="0">
+        <v>2.0</v>
+      </c>
+      <c r="B3" t="s" s="0">
+        <v>5</v>
+      </c>
+      <c r="C3" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="D3" t="s" s="0">
+        <v>7</v>
+      </c>
+      <c r="E3" t="s" s="0">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n" s="0">
+        <v>3.0</v>
+      </c>
+      <c r="B4" t="s" s="0">
+        <v>9</v>
+      </c>
+      <c r="C4" t="s" s="0">
+        <v>10</v>
+      </c>
+      <c r="D4" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="E4" t="s" s="0">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n" s="0">
+        <v>4.0</v>
+      </c>
+      <c r="B5" t="s" s="0">
+        <v>13</v>
+      </c>
+      <c r="C5" t="s" s="0">
+        <v>10</v>
+      </c>
+      <c r="D5" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="E5" t="s" s="0">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n" s="0">
+        <v>5.0</v>
+      </c>
+      <c r="B6" t="s" s="0">
+        <v>5</v>
+      </c>
+      <c r="C6" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="D6" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="E6" t="s" s="0">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n" s="0">
+        <v>6.0</v>
+      </c>
+      <c r="B7" t="s" s="0">
+        <v>5</v>
+      </c>
+      <c r="C7" t="s" s="0">
+        <v>14</v>
+      </c>
+      <c r="D7" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="E7" t="s" s="0">
+        <v>12</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>